<commit_message>
Organización estructura y definición Clase Excel para lectura y Escritura
</commit_message>
<xml_diff>
--- a/src/main/resources/outputData.xlsx
+++ b/src/main/resources/outputData.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="4">
   <si>
     <t>Iphone</t>
   </si>
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A4674D-028E-DD41-B3CC-0F291AEDE1AC}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -439,6 +439,40 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>